<commit_message>
The functionality to get system list from file was implemented.
</commit_message>
<xml_diff>
--- a/Mosquito/mosdb.xlsx
+++ b/Mosquito/mosdb.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="15315" windowHeight="6210" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="15315" windowHeight="6210" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Системы" sheetId="10" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="95">
   <si>
     <t>Имя</t>
   </si>
@@ -306,6 +306,12 @@
   </si>
   <si>
     <t>25-ая система</t>
+  </si>
+  <si>
+    <t>Системы</t>
+  </si>
+  <si>
+    <t>Тестовая</t>
   </si>
 </sst>
 </file>
@@ -663,10 +669,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -690,6 +696,14 @@
         <v>92</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>94</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -697,19 +711,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D2" sqref="D2:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="49.28515625" customWidth="1"/>
     <col min="3" max="3" width="18.28515625" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>91</v>
       </c>
@@ -719,8 +734,11 @@
       <c r="C1" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -730,8 +748,11 @@
       <c r="C2" s="2">
         <v>21.2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -741,8 +762,11 @@
       <c r="C3" s="2">
         <v>21.3</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -752,8 +776,11 @@
       <c r="C4" s="2">
         <v>23.1</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -764,7 +791,7 @@
         <v>23.2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -774,8 +801,11 @@
       <c r="C6" s="2">
         <v>35.5</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -784,6 +814,9 @@
       </c>
       <c r="C7" s="2">
         <v>36.6</v>
+      </c>
+      <c r="D7">
+        <v>1.2</v>
       </c>
     </row>
   </sheetData>
@@ -794,19 +827,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="46.85546875" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>91</v>
       </c>
@@ -816,8 +850,11 @@
       <c r="C1" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -827,8 +864,11 @@
       <c r="C2" s="2">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -838,8 +878,11 @@
       <c r="C3" s="2">
         <v>26.1</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -849,8 +892,11 @@
       <c r="C4" s="2">
         <v>26.5</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -861,7 +907,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
     </row>
@@ -872,19 +918,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="D2" sqref="D2:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="54.42578125" customWidth="1"/>
     <col min="3" max="3" width="14.85546875" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>91</v>
       </c>
@@ -894,8 +941,11 @@
       <c r="C1" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -905,8 +955,11 @@
       <c r="C2" s="2">
         <v>37</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -916,8 +969,11 @@
       <c r="C3" s="2">
         <v>37.5</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -927,8 +983,11 @@
       <c r="C4" s="2">
         <v>40</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -939,7 +998,7 @@
         <v>40.299999999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -949,8 +1008,11 @@
       <c r="C6" s="2">
         <v>35</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -960,8 +1022,11 @@
       <c r="C7" s="2">
         <v>35.5</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -971,8 +1036,11 @@
       <c r="C8" s="2">
         <v>38.6</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -983,7 +1051,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -993,8 +1061,11 @@
       <c r="C10" s="2">
         <v>55.3</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1004,8 +1075,11 @@
       <c r="C11" s="2">
         <v>58</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1014,6 +1088,9 @@
       </c>
       <c r="C12" s="2">
         <v>90</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1023,19 +1100,20 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="D2" sqref="D2:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="51.7109375" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>91</v>
       </c>
@@ -1045,8 +1123,11 @@
       <c r="C1" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1056,8 +1137,11 @@
       <c r="C2">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1067,8 +1151,11 @@
       <c r="C3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1078,8 +1165,11 @@
       <c r="C4">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1097,19 +1187,20 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="D2" sqref="D2:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="45.42578125" customWidth="1"/>
     <col min="3" max="3" width="17.7109375" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>91</v>
       </c>
@@ -1119,8 +1210,11 @@
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1130,8 +1224,11 @@
       <c r="C2" s="2">
         <v>2.1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1140,10 +1237,13 @@
       </c>
       <c r="C3" s="2">
         <f t="shared" ref="C3:C5" ca="1" si="0">RANDBETWEEN(50,300)/100</f>
-        <v>1.23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.83</v>
+      </c>
+      <c r="D3">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1152,10 +1252,13 @@
       </c>
       <c r="C4" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.94</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1.17</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1164,10 +1267,10 @@
       </c>
       <c r="C5" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1.17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1176,10 +1279,13 @@
       </c>
       <c r="C6" s="2">
         <f ca="1">RANDBETWEEN(50,300)/100</f>
-        <v>2.0299999999999998</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1188,10 +1294,13 @@
       </c>
       <c r="C7" s="2">
         <f ca="1">RANDBETWEEN(50,300)/100</f>
-        <v>0.79</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="D7">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1200,7 +1309,10 @@
       </c>
       <c r="C8" s="2">
         <f ca="1">RANDBETWEEN(50,300)/100</f>
-        <v>0.73</v>
+        <v>0.77</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1210,19 +1322,20 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="48.7109375" customWidth="1"/>
     <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>91</v>
       </c>
@@ -1232,8 +1345,11 @@
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1242,10 +1358,13 @@
       </c>
       <c r="C2" s="2">
         <f ca="1">RANDBETWEEN(50,300)/100</f>
-        <v>2.38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2.42</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1254,10 +1373,13 @@
       </c>
       <c r="C3" s="2">
         <f ca="1">RANDBETWEEN(50,300)/100</f>
-        <v>1.8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="D3">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1266,10 +1388,13 @@
       </c>
       <c r="C4" s="2">
         <f ca="1">RANDBETWEEN(50,300)/100</f>
-        <v>2.42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1.49</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1278,10 +1403,10 @@
       </c>
       <c r="C5" s="2">
         <f ca="1">RANDBETWEEN(50,300)/100</f>
-        <v>0.52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1291,8 +1416,11 @@
       <c r="C6" s="2">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1301,7 +1429,10 @@
       </c>
       <c r="C7" s="2">
         <f ca="1">RANDBETWEEN(50,300)/100</f>
-        <v>2.5099999999999998</v>
+        <v>1.83</v>
+      </c>
+      <c r="D7">
+        <v>1.2</v>
       </c>
     </row>
   </sheetData>
@@ -1311,19 +1442,20 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C54"/>
+  <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="58.5703125" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>91</v>
       </c>
@@ -1333,8 +1465,11 @@
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1344,8 +1479,11 @@
       <c r="C2" s="2">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1354,10 +1492,13 @@
       </c>
       <c r="C3" s="2">
         <f t="shared" ref="C3:C40" ca="1" si="0">RANDBETWEEN(50,300)/100</f>
-        <v>1.29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2.59</v>
+      </c>
+      <c r="D3">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1366,10 +1507,13 @@
       </c>
       <c r="C4" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.2000000000000002</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2.06</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1378,10 +1522,10 @@
       </c>
       <c r="C5" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2.58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1390,10 +1534,13 @@
       </c>
       <c r="C6" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.84</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1402,10 +1549,13 @@
       </c>
       <c r="C7" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.75</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2.25</v>
+      </c>
+      <c r="D7">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1414,10 +1564,13 @@
       </c>
       <c r="C8" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.78</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1.36</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1426,10 +1579,10 @@
       </c>
       <c r="C9" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2.0699999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1438,10 +1591,13 @@
       </c>
       <c r="C10" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2.57</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1450,10 +1606,13 @@
       </c>
       <c r="C11" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.43</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="D11">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1462,10 +1621,13 @@
       </c>
       <c r="C12" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.68</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1.75</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1474,10 +1636,10 @@
       </c>
       <c r="C13" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.64</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1486,10 +1648,13 @@
       </c>
       <c r="C14" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.4500000000000002</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.61</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1498,10 +1663,13 @@
       </c>
       <c r="C15" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1.46</v>
+      </c>
+      <c r="D15">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1510,10 +1678,13 @@
       </c>
       <c r="C16" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.48</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2.06</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1522,10 +1693,10 @@
       </c>
       <c r="C17" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1.84</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1534,10 +1705,13 @@
       </c>
       <c r="C18" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.38</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1.77</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1546,10 +1720,13 @@
       </c>
       <c r="C19" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.79</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2.19</v>
+      </c>
+      <c r="D19">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1558,10 +1735,13 @@
       </c>
       <c r="C20" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.62</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2.54</v>
+      </c>
+      <c r="D20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1570,10 +1750,10 @@
       </c>
       <c r="C21" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.87</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1582,10 +1762,13 @@
       </c>
       <c r="C22" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.63</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.75</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1594,10 +1777,13 @@
       </c>
       <c r="C23" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2.9</v>
+      </c>
+      <c r="D23">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1606,10 +1792,13 @@
       </c>
       <c r="C24" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.06</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.74</v>
+      </c>
+      <c r="D24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1618,10 +1807,10 @@
       </c>
       <c r="C25" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.56</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1.58</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1630,10 +1819,13 @@
       </c>
       <c r="C26" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.72</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2.92</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1642,10 +1834,13 @@
       </c>
       <c r="C27" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.76</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2.15</v>
+      </c>
+      <c r="D27">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1654,10 +1849,13 @@
       </c>
       <c r="C28" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.75</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1.99</v>
+      </c>
+      <c r="D28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1666,10 +1864,10 @@
       </c>
       <c r="C29" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.4500000000000002</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2.63</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1678,10 +1876,13 @@
       </c>
       <c r="C30" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.73</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1.23</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1690,10 +1891,13 @@
       </c>
       <c r="C31" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.54</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1.37</v>
+      </c>
+      <c r="D31">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1702,10 +1906,13 @@
       </c>
       <c r="C32" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.91</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1.41</v>
+      </c>
+      <c r="D32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1714,10 +1921,10 @@
       </c>
       <c r="C33" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.1399999999999999</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1.72</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1726,10 +1933,13 @@
       </c>
       <c r="C34" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.57</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.63</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1738,10 +1948,13 @@
       </c>
       <c r="C35" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.4700000000000002</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2.82</v>
+      </c>
+      <c r="D35">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1750,10 +1963,13 @@
       </c>
       <c r="C36" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.2999999999999998</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2.16</v>
+      </c>
+      <c r="D36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1762,10 +1978,10 @@
       </c>
       <c r="C37" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.72</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1774,10 +1990,13 @@
       </c>
       <c r="C38" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.69</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1.22</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1786,10 +2005,13 @@
       </c>
       <c r="C39" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.95</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2.34</v>
+      </c>
+      <c r="D39">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1798,7 +2020,10 @@
       </c>
       <c r="C40" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.41</v>
+        <v>2.54</v>
+      </c>
+      <c r="D40">
+        <v>2</v>
       </c>
     </row>
     <row r="54" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
add system elements on form
</commit_message>
<xml_diff>
--- a/Mosquito/mosdb.xlsx
+++ b/Mosquito/mosdb.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\!Mosquito\Mosquito\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="15315" windowHeight="6210" activeTab="7"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="15315" windowHeight="6210"/>
   </bookViews>
   <sheets>
     <sheet name="Системы" sheetId="10" r:id="rId1"/>
@@ -22,7 +17,7 @@
     <sheet name="Дополнительные детали" sheetId="5" r:id="rId8"/>
     <sheet name="Настройки" sheetId="6" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -425,7 +420,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -460,7 +455,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -671,7 +666,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -1103,7 +1098,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D5"/>
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1237,7 +1232,7 @@
       </c>
       <c r="C3" s="2">
         <f t="shared" ref="C3:C5" ca="1" si="0">RANDBETWEEN(50,300)/100</f>
-        <v>0.83</v>
+        <v>2.0099999999999998</v>
       </c>
       <c r="D3">
         <v>1.2</v>
@@ -1252,7 +1247,7 @@
       </c>
       <c r="C4" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.17</v>
+        <v>0.63</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -1267,7 +1262,7 @@
       </c>
       <c r="C5" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.17</v>
+        <v>1.91</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1294,7 +1289,7 @@
       </c>
       <c r="C7" s="2">
         <f ca="1">RANDBETWEEN(50,300)/100</f>
-        <v>2.0099999999999998</v>
+        <v>2.99</v>
       </c>
       <c r="D7">
         <v>1.2</v>
@@ -1309,7 +1304,7 @@
       </c>
       <c r="C8" s="2">
         <f ca="1">RANDBETWEEN(50,300)/100</f>
-        <v>0.77</v>
+        <v>1.51</v>
       </c>
       <c r="D8">
         <v>2</v>
@@ -1358,7 +1353,7 @@
       </c>
       <c r="C2" s="2">
         <f ca="1">RANDBETWEEN(50,300)/100</f>
-        <v>2.42</v>
+        <v>2.2599999999999998</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1373,7 +1368,7 @@
       </c>
       <c r="C3" s="2">
         <f ca="1">RANDBETWEEN(50,300)/100</f>
-        <v>1.1299999999999999</v>
+        <v>0.99</v>
       </c>
       <c r="D3">
         <v>1.2</v>
@@ -1388,7 +1383,7 @@
       </c>
       <c r="C4" s="2">
         <f ca="1">RANDBETWEEN(50,300)/100</f>
-        <v>1.49</v>
+        <v>2.6</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -1403,7 +1398,7 @@
       </c>
       <c r="C5" s="2">
         <f ca="1">RANDBETWEEN(50,300)/100</f>
-        <v>0.68</v>
+        <v>2.06</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1429,7 +1424,7 @@
       </c>
       <c r="C7" s="2">
         <f ca="1">RANDBETWEEN(50,300)/100</f>
-        <v>1.83</v>
+        <v>2.54</v>
       </c>
       <c r="D7">
         <v>1.2</v>
@@ -1444,7 +1439,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
@@ -1492,7 +1487,7 @@
       </c>
       <c r="C3" s="2">
         <f t="shared" ref="C3:C40" ca="1" si="0">RANDBETWEEN(50,300)/100</f>
-        <v>2.59</v>
+        <v>1.37</v>
       </c>
       <c r="D3">
         <v>1.2</v>
@@ -1507,7 +1502,7 @@
       </c>
       <c r="C4" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.06</v>
+        <v>1.19</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -1522,7 +1517,7 @@
       </c>
       <c r="C5" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.58</v>
+        <v>1.67</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1534,7 +1529,7 @@
       </c>
       <c r="C6" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.5</v>
+        <v>0.94</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -1549,7 +1544,7 @@
       </c>
       <c r="C7" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.25</v>
+        <v>1.58</v>
       </c>
       <c r="D7">
         <v>1.2</v>
@@ -1564,7 +1559,7 @@
       </c>
       <c r="C8" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.36</v>
+        <v>2.2599999999999998</v>
       </c>
       <c r="D8">
         <v>2</v>
@@ -1579,7 +1574,7 @@
       </c>
       <c r="C9" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.0699999999999998</v>
+        <v>1.35</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1591,7 +1586,7 @@
       </c>
       <c r="C10" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.57</v>
+        <v>0.95</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -1606,7 +1601,7 @@
       </c>
       <c r="C11" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.3199999999999998</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="D11">
         <v>1.2</v>
@@ -1621,7 +1616,7 @@
       </c>
       <c r="C12" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.75</v>
+        <v>2.2200000000000002</v>
       </c>
       <c r="D12">
         <v>2</v>
@@ -1636,7 +1631,7 @@
       </c>
       <c r="C13" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.6</v>
+        <v>2.91</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1648,7 +1643,7 @@
       </c>
       <c r="C14" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.61</v>
+        <v>2.4700000000000002</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -1663,7 +1658,7 @@
       </c>
       <c r="C15" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.46</v>
+        <v>2.0099999999999998</v>
       </c>
       <c r="D15">
         <v>1.2</v>
@@ -1678,7 +1673,7 @@
       </c>
       <c r="C16" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.06</v>
+        <v>0.66</v>
       </c>
       <c r="D16">
         <v>2</v>
@@ -1693,7 +1688,7 @@
       </c>
       <c r="C17" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.84</v>
+        <v>1.88</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1705,7 +1700,7 @@
       </c>
       <c r="C18" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.77</v>
+        <v>2.6</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -1720,7 +1715,7 @@
       </c>
       <c r="C19" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.19</v>
+        <v>2.3199999999999998</v>
       </c>
       <c r="D19">
         <v>1.2</v>
@@ -1735,7 +1730,7 @@
       </c>
       <c r="C20" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.54</v>
+        <v>1.33</v>
       </c>
       <c r="D20">
         <v>2</v>
@@ -1750,7 +1745,7 @@
       </c>
       <c r="C21" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.25</v>
+        <v>1.35</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1762,7 +1757,7 @@
       </c>
       <c r="C22" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.75</v>
+        <v>2.37</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -1777,7 +1772,7 @@
       </c>
       <c r="C23" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.9</v>
+        <v>0.72</v>
       </c>
       <c r="D23">
         <v>1.2</v>
@@ -1792,7 +1787,7 @@
       </c>
       <c r="C24" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.74</v>
+        <v>2.48</v>
       </c>
       <c r="D24">
         <v>2</v>
@@ -1807,7 +1802,7 @@
       </c>
       <c r="C25" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.58</v>
+        <v>1.19</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1819,7 +1814,7 @@
       </c>
       <c r="C26" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.92</v>
+        <v>1.29</v>
       </c>
       <c r="D26">
         <v>1</v>
@@ -1834,7 +1829,7 @@
       </c>
       <c r="C27" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.15</v>
+        <v>0.95</v>
       </c>
       <c r="D27">
         <v>1.2</v>
@@ -1849,7 +1844,7 @@
       </c>
       <c r="C28" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.99</v>
+        <v>1.06</v>
       </c>
       <c r="D28">
         <v>2</v>
@@ -1864,7 +1859,7 @@
       </c>
       <c r="C29" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.63</v>
+        <v>0.91</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1876,7 +1871,7 @@
       </c>
       <c r="C30" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.23</v>
+        <v>0.8</v>
       </c>
       <c r="D30">
         <v>1</v>
@@ -1891,7 +1886,7 @@
       </c>
       <c r="C31" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.37</v>
+        <v>1.33</v>
       </c>
       <c r="D31">
         <v>1.2</v>
@@ -1906,7 +1901,7 @@
       </c>
       <c r="C32" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.41</v>
+        <v>0.76</v>
       </c>
       <c r="D32">
         <v>2</v>
@@ -1921,7 +1916,7 @@
       </c>
       <c r="C33" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.72</v>
+        <v>1.52</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1933,7 +1928,7 @@
       </c>
       <c r="C34" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.63</v>
+        <v>1.51</v>
       </c>
       <c r="D34">
         <v>1</v>
@@ -1948,7 +1943,7 @@
       </c>
       <c r="C35" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.82</v>
+        <v>2.02</v>
       </c>
       <c r="D35">
         <v>1.2</v>
@@ -1963,7 +1958,7 @@
       </c>
       <c r="C36" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.16</v>
+        <v>1.07</v>
       </c>
       <c r="D36">
         <v>2</v>
@@ -1978,7 +1973,7 @@
       </c>
       <c r="C37" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.74</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1990,7 +1985,7 @@
       </c>
       <c r="C38" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.22</v>
+        <v>2.25</v>
       </c>
       <c r="D38">
         <v>1</v>
@@ -2005,7 +2000,7 @@
       </c>
       <c r="C39" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.34</v>
+        <v>2.25</v>
       </c>
       <c r="D39">
         <v>1.2</v>
@@ -2020,7 +2015,7 @@
       </c>
       <c r="C40" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.54</v>
+        <v>2.44</v>
       </c>
       <c r="D40">
         <v>2</v>

</xml_diff>

<commit_message>
added on setting glue
</commit_message>
<xml_diff>
--- a/Mosquito/mosdb.xlsx
+++ b/Mosquito/mosdb.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="15315" windowHeight="6210"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="15315" windowHeight="6210" firstSheet="1" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Системы" sheetId="10" r:id="rId1"/>
@@ -14,15 +14,17 @@
     <sheet name="Шнуры" sheetId="4" r:id="rId5"/>
     <sheet name="Уголки" sheetId="7" r:id="rId6"/>
     <sheet name="Крепления" sheetId="8" r:id="rId7"/>
-    <sheet name="Дополнительные детали" sheetId="5" r:id="rId8"/>
-    <sheet name="Настройки" sheetId="6" r:id="rId9"/>
+    <sheet name="Кремпления поперечины" sheetId="11" r:id="rId8"/>
+    <sheet name="Ручки" sheetId="12" r:id="rId9"/>
+    <sheet name="Дополнительные детали" sheetId="5" r:id="rId10"/>
+    <sheet name="Настройки" sheetId="6" r:id="rId11"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="98">
   <si>
     <t>Имя</t>
   </si>
@@ -307,6 +309,15 @@
   </si>
   <si>
     <t>Тестовая</t>
+  </si>
+  <si>
+    <t>Стоимость клея (1 тюбик)</t>
+  </si>
+  <si>
+    <t>Количество сетей, обслуживаемые одним тюбиком клея</t>
+  </si>
+  <si>
+    <t>шт.</t>
   </si>
 </sst>
 </file>
@@ -352,7 +363,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -360,6 +371,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -666,7 +680,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -701,6 +715,588 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D54"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="58.5703125" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f>A2+1</f>
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="2">
+        <f t="shared" ref="C3:C28" ca="1" si="0">RANDBETWEEN(50,300)/100</f>
+        <v>1.94</v>
+      </c>
+      <c r="D3">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f t="shared" ref="A4:A28" si="1">A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.31</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.89</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.35</v>
+      </c>
+      <c r="D7">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.73</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.95</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.69</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.62</v>
+      </c>
+      <c r="D11">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.94</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.39</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C15" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.62</v>
+      </c>
+      <c r="D15">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C16" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.38</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.41</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.78</v>
+      </c>
+      <c r="D19">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.14</v>
+      </c>
+      <c r="D20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C22" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.58</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C23" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.84</v>
+      </c>
+      <c r="D23">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C24" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.25</v>
+      </c>
+      <c r="D24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C25" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C26" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.76</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C27" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D27">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C28" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.36</v>
+      </c>
+      <c r="D28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B54" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="56.5703125" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2">
+        <v>50</v>
+      </c>
+      <c r="D2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C5">
+        <v>60</v>
+      </c>
+      <c r="D5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C6">
+        <v>48</v>
+      </c>
+      <c r="D6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C7">
+        <v>15</v>
+      </c>
+      <c r="D7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C8">
+        <v>50</v>
+      </c>
+      <c r="D8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1232,7 +1828,7 @@
       </c>
       <c r="C3" s="2">
         <f t="shared" ref="C3:C5" ca="1" si="0">RANDBETWEEN(50,300)/100</f>
-        <v>2.0099999999999998</v>
+        <v>2.1</v>
       </c>
       <c r="D3">
         <v>1.2</v>
@@ -1247,7 +1843,7 @@
       </c>
       <c r="C4" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.63</v>
+        <v>2.96</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -1262,7 +1858,7 @@
       </c>
       <c r="C5" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.91</v>
+        <v>1.39</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1274,7 +1870,7 @@
       </c>
       <c r="C6" s="2">
         <f ca="1">RANDBETWEEN(50,300)/100</f>
-        <v>2.4700000000000002</v>
+        <v>1.73</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -1289,7 +1885,7 @@
       </c>
       <c r="C7" s="2">
         <f ca="1">RANDBETWEEN(50,300)/100</f>
-        <v>2.99</v>
+        <v>2.97</v>
       </c>
       <c r="D7">
         <v>1.2</v>
@@ -1304,7 +1900,7 @@
       </c>
       <c r="C8" s="2">
         <f ca="1">RANDBETWEEN(50,300)/100</f>
-        <v>1.51</v>
+        <v>0.84</v>
       </c>
       <c r="D8">
         <v>2</v>
@@ -1317,10 +1913,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1353,7 +1949,7 @@
       </c>
       <c r="C2" s="2">
         <f ca="1">RANDBETWEEN(50,300)/100</f>
-        <v>2.2599999999999998</v>
+        <v>2.58</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1368,7 +1964,7 @@
       </c>
       <c r="C3" s="2">
         <f ca="1">RANDBETWEEN(50,300)/100</f>
-        <v>0.99</v>
+        <v>1.42</v>
       </c>
       <c r="D3">
         <v>1.2</v>
@@ -1383,7 +1979,7 @@
       </c>
       <c r="C4" s="2">
         <f ca="1">RANDBETWEEN(50,300)/100</f>
-        <v>2.6</v>
+        <v>1.04</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -1398,36 +1994,7 @@
       </c>
       <c r="C5" s="2">
         <f ca="1">RANDBETWEEN(50,300)/100</f>
-        <v>2.06</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" s="2">
-        <v>0.75</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" s="2">
-        <f ca="1">RANDBETWEEN(50,300)/100</f>
-        <v>2.54</v>
-      </c>
-      <c r="D7">
-        <v>1.2</v>
+        <v>1.05</v>
       </c>
     </row>
   </sheetData>
@@ -1437,17 +2004,16 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D54"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="58.5703125" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" customWidth="1"/>
-    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="2" max="2" width="42.28515625" customWidth="1"/>
+    <col min="3" max="4" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1469,7 +2035,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C2" s="2">
         <v>0.75</v>
@@ -1483,546 +2049,15 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C3" s="2">
-        <f t="shared" ref="C3:C40" ca="1" si="0">RANDBETWEEN(50,300)/100</f>
-        <v>1.37</v>
+        <f ca="1">RANDBETWEEN(50,300)/100</f>
+        <v>2.9</v>
       </c>
       <c r="D3">
         <v>1.2</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.19</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C5" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.67</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.94</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C7" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.58</v>
-      </c>
-      <c r="D7">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.2599999999999998</v>
-      </c>
-      <c r="D8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C10" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.95</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C11" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="D11">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C12" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.2200000000000002</v>
-      </c>
-      <c r="D12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C13" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.91</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C14" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.4700000000000002</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C15" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.0099999999999998</v>
-      </c>
-      <c r="D15">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C16" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.66</v>
-      </c>
-      <c r="D16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C17" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.88</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C18" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.6</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C19" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="D19">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C20" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.33</v>
-      </c>
-      <c r="D20">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C21" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.35</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>21</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C22" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.37</v>
-      </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>22</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C23" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.72</v>
-      </c>
-      <c r="D23">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>23</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C24" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.48</v>
-      </c>
-      <c r="D24">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>24</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C25" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.19</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>25</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C26" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.29</v>
-      </c>
-      <c r="D26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>26</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C27" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.95</v>
-      </c>
-      <c r="D27">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>27</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C28" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.06</v>
-      </c>
-      <c r="D28">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>28</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C29" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.91</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>29</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C30" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.8</v>
-      </c>
-      <c r="D30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>30</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C31" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.33</v>
-      </c>
-      <c r="D31">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>31</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C32" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.76</v>
-      </c>
-      <c r="D32">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>32</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C33" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.52</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>33</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C34" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.51</v>
-      </c>
-      <c r="D34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>34</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C35" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.02</v>
-      </c>
-      <c r="D35">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>35</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C36" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.07</v>
-      </c>
-      <c r="D36">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>36</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C37" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.9</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>37</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C38" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.25</v>
-      </c>
-      <c r="D38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>38</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C39" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.25</v>
-      </c>
-      <c r="D39">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>39</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C40" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.44</v>
-      </c>
-      <c r="D40">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B54" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2031,17 +2066,17 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="34.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.140625" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -2049,87 +2084,198 @@
         <v>91</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>4</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C2">
-        <v>50</v>
-      </c>
-      <c r="D2" t="s">
-        <v>84</v>
+      <c r="B2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="2">
+        <f t="shared" ref="C2:C13" ca="1" si="0">RANDBETWEEN(50,300)/100</f>
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="D2">
+        <v>1.2</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C3">
-        <v>15</v>
-      </c>
-      <c r="D3" t="s">
-        <v>86</v>
+        <f>A2+1</f>
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.88</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
+        <f t="shared" ref="A4:A13" si="1">A3+1</f>
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>87</v>
-      </c>
-      <c r="C4">
-        <v>20</v>
-      </c>
-      <c r="D4" t="s">
-        <v>84</v>
+      <c r="B4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.85</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C5">
-        <v>60</v>
-      </c>
-      <c r="D5" t="s">
-        <v>89</v>
+      <c r="B5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.74</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>90</v>
-      </c>
-      <c r="C6">
-        <v>48</v>
-      </c>
-      <c r="D6" t="s">
-        <v>89</v>
+      <c r="B6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="D6">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.33</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.74</v>
+      </c>
+      <c r="D10">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.38</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.53</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Some product attributes were added.
</commit_message>
<xml_diff>
--- a/Mosquito/mosdb.xlsx
+++ b/Mosquito/mosdb.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\!Mosquito\Mosquito\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="15315" windowHeight="6210" firstSheet="1" activeTab="10"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="15315" windowHeight="6210" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Системы" sheetId="10" r:id="rId1"/>
@@ -17,14 +22,15 @@
     <sheet name="Кремпления поперечины" sheetId="11" r:id="rId8"/>
     <sheet name="Ручки" sheetId="12" r:id="rId9"/>
     <sheet name="Дополнительные детали" sheetId="5" r:id="rId10"/>
-    <sheet name="Настройки" sheetId="6" r:id="rId11"/>
+    <sheet name="Комплектующие детали" sheetId="13" r:id="rId11"/>
+    <sheet name="Настройки" sheetId="6" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="102">
   <si>
     <t>Имя</t>
   </si>
@@ -318,6 +324,18 @@
   </si>
   <si>
     <t>шт.</t>
+  </si>
+  <si>
+    <t>Заклёпки</t>
+  </si>
+  <si>
+    <t>Размер</t>
+  </si>
+  <si>
+    <t>Количество</t>
+  </si>
+  <si>
+    <t>Заклёпки (шт)</t>
   </si>
 </sst>
 </file>
@@ -434,7 +452,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -469,7 +487,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -681,7 +699,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -720,14 +738,15 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D54"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A28"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="58.5703125" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
@@ -749,48 +768,50 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
+        <f>1</f>
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="C2" s="2">
-        <v>0.75</v>
+        <f t="shared" ref="C2:C25" ca="1" si="0">RANDBETWEEN(50,300)/100</f>
+        <v>2.84</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
-        <f>A2+1</f>
+        <f t="shared" ref="A3:A24" si="1">A2+1</f>
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C3" s="2">
-        <f t="shared" ref="C3:C28" ca="1" si="0">RANDBETWEEN(50,300)/100</f>
-        <v>1.94</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>2.31</v>
       </c>
       <c r="D3">
-        <v>1.2</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ref="A4:A28" si="1">A3+1</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C4" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.31</v>
+        <v>2.1</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -799,11 +820,14 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C5" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.35</v>
+        <v>1.4</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -812,14 +836,14 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C6" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.89</v>
+        <v>1.99</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -828,14 +852,14 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C7" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.35</v>
+        <v>2.14</v>
       </c>
       <c r="D7">
-        <v>1.2</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -844,14 +868,11 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C8" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.73</v>
-      </c>
-      <c r="D8">
-        <v>2</v>
+        <v>0.82</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -860,11 +881,14 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C9" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.95</v>
+        <v>2.91</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -873,14 +897,14 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="C10" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.69</v>
+        <v>1.83</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -889,14 +913,14 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C11" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.62</v>
+        <v>0.72</v>
       </c>
       <c r="D11">
-        <v>1.2</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -905,14 +929,11 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C12" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.94</v>
-      </c>
-      <c r="D12">
-        <v>2</v>
+        <v>1.64</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -921,11 +942,14 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C13" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.59</v>
+        <v>0.97</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -934,14 +958,14 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C14" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.39</v>
+        <v>2.63</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -950,14 +974,14 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C15" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.62</v>
+        <v>1.85</v>
       </c>
       <c r="D15">
-        <v>1.2</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -966,11 +990,11 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C16" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.38</v>
+        <v>2.95</v>
       </c>
       <c r="D16">
         <v>2</v>
@@ -982,11 +1006,14 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C17" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.76</v>
+        <v>0.65</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -995,14 +1022,14 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C18" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.41</v>
+        <v>1.75</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1011,14 +1038,14 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C19" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.78</v>
+        <v>1.39</v>
       </c>
       <c r="D19">
-        <v>1.2</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1027,14 +1054,11 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C20" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.14</v>
-      </c>
-      <c r="D20">
-        <v>2</v>
+        <v>1.26</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1043,11 +1067,14 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C21" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.6</v>
+        <v>0.5</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1056,14 +1083,14 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C22" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.58</v>
+        <v>0.8</v>
       </c>
       <c r="D22">
-        <v>1</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1072,14 +1099,14 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C23" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.84</v>
+        <v>0.61</v>
       </c>
       <c r="D23">
-        <v>1.2</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1088,79 +1115,30 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C24" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.25</v>
-      </c>
-      <c r="D24">
-        <v>2</v>
+        <v>1.67</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
-        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C25" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.62</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <f t="shared" si="1"/>
-        <v>25</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C26" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.76</v>
-      </c>
-      <c r="D26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <f t="shared" si="1"/>
-        <v>26</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C27" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="D27">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <f t="shared" si="1"/>
-        <v>27</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C28" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.36</v>
-      </c>
-      <c r="D28">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B54" s="1"/>
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="D25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B51" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1169,10 +1147,52 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="27.7109375" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2">
+        <v>1.45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1305,7 +1325,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D5"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1421,7 +1441,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D5"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1509,10 +1529,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D5"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1520,9 +1540,10 @@
     <col min="2" max="2" width="54.42578125" customWidth="1"/>
     <col min="3" max="3" width="14.85546875" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>91</v>
       </c>
@@ -1535,8 +1556,11 @@
       <c r="D1" s="3" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1549,10 +1573,13 @@
       <c r="D2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>17</v>
@@ -1563,10 +1590,13 @@
       <c r="D3">
         <v>1.2</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>18</v>
@@ -1577,10 +1607,13 @@
       <c r="D4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>19</v>
@@ -1588,10 +1621,13 @@
       <c r="C5" s="2">
         <v>40.299999999999997</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>20</v>
@@ -1602,10 +1638,13 @@
       <c r="D6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>21</v>
@@ -1616,10 +1655,13 @@
       <c r="D7">
         <v>1.2</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>22</v>
@@ -1630,10 +1672,13 @@
       <c r="D8">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>23</v>
@@ -1641,10 +1686,13 @@
       <c r="C9" s="2">
         <v>50</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>24</v>
@@ -1655,10 +1703,13 @@
       <c r="D10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>25</v>
@@ -1669,10 +1720,13 @@
       <c r="D11">
         <v>1.2</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>26</v>
@@ -1682,6 +1736,9 @@
       </c>
       <c r="D12">
         <v>2</v>
+      </c>
+      <c r="E12">
+        <v>1400</v>
       </c>
     </row>
   </sheetData>
@@ -1778,10 +1835,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1789,9 +1846,11 @@
     <col min="2" max="2" width="45.42578125" customWidth="1"/>
     <col min="3" max="3" width="17.7109375" customWidth="1"/>
     <col min="4" max="4" width="17.28515625" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" customWidth="1"/>
+    <col min="6" max="6" width="38.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>91</v>
       </c>
@@ -1804,8 +1863,14 @@
       <c r="D1" s="3" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1818,8 +1883,14 @@
       <c r="D2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>4</v>
+      </c>
+      <c r="F2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1828,13 +1899,19 @@
       </c>
       <c r="C3" s="2">
         <f t="shared" ref="C3:C5" ca="1" si="0">RANDBETWEEN(50,300)/100</f>
-        <v>2.1</v>
+        <v>2.59</v>
       </c>
       <c r="D3">
         <v>1.2</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>4</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1843,13 +1920,19 @@
       </c>
       <c r="C4" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.96</v>
+        <v>0.9</v>
       </c>
       <c r="D4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1858,10 +1941,16 @@
       </c>
       <c r="C5" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.6</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1870,13 +1959,19 @@
       </c>
       <c r="C6" s="2">
         <f ca="1">RANDBETWEEN(50,300)/100</f>
-        <v>1.73</v>
+        <v>1.87</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1885,13 +1980,19 @@
       </c>
       <c r="C7" s="2">
         <f ca="1">RANDBETWEEN(50,300)/100</f>
-        <v>2.97</v>
+        <v>2.2200000000000002</v>
       </c>
       <c r="D7">
         <v>1.2</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>4</v>
+      </c>
+      <c r="F7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1900,10 +2001,16 @@
       </c>
       <c r="C8" s="2">
         <f ca="1">RANDBETWEEN(50,300)/100</f>
-        <v>0.84</v>
+        <v>1.68</v>
       </c>
       <c r="D8">
         <v>2</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1916,7 +2023,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1949,7 +2056,7 @@
       </c>
       <c r="C2" s="2">
         <f ca="1">RANDBETWEEN(50,300)/100</f>
-        <v>2.58</v>
+        <v>2.5099999999999998</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1964,7 +2071,7 @@
       </c>
       <c r="C3" s="2">
         <f ca="1">RANDBETWEEN(50,300)/100</f>
-        <v>1.42</v>
+        <v>2.68</v>
       </c>
       <c r="D3">
         <v>1.2</v>
@@ -1979,7 +2086,7 @@
       </c>
       <c r="C4" s="2">
         <f ca="1">RANDBETWEEN(50,300)/100</f>
-        <v>1.04</v>
+        <v>2.67</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -1994,7 +2101,7 @@
       </c>
       <c r="C5" s="2">
         <f ca="1">RANDBETWEEN(50,300)/100</f>
-        <v>1.05</v>
+        <v>2.95</v>
       </c>
     </row>
   </sheetData>
@@ -2053,7 +2160,7 @@
       </c>
       <c r="C3" s="2">
         <f ca="1">RANDBETWEEN(50,300)/100</f>
-        <v>2.9</v>
+        <v>2.66</v>
       </c>
       <c r="D3">
         <v>1.2</v>
@@ -2066,15 +2173,15 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="32.140625" customWidth="1"/>
+    <col min="2" max="2" width="58.5703125" customWidth="1"/>
     <col min="3" max="3" width="26.140625" customWidth="1"/>
     <col min="4" max="4" width="15.28515625" customWidth="1"/>
   </cols>
@@ -2102,7 +2209,7 @@
       </c>
       <c r="C2" s="2">
         <f t="shared" ref="C2:C13" ca="1" si="0">RANDBETWEEN(50,300)/100</f>
-        <v>2.0299999999999998</v>
+        <v>2.96</v>
       </c>
       <c r="D2">
         <v>1.2</v>
@@ -2118,7 +2225,7 @@
       </c>
       <c r="C3" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.88</v>
+        <v>1.95</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -2126,7 +2233,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ref="A4:A13" si="1">A3+1</f>
+        <f t="shared" ref="A4:A15" si="1">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -2134,7 +2241,7 @@
       </c>
       <c r="C4" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.85</v>
+        <v>2.77</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2147,7 +2254,7 @@
       </c>
       <c r="C5" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.74</v>
+        <v>1.75</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -2163,7 +2270,7 @@
       </c>
       <c r="C6" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.0099999999999998</v>
+        <v>2.42</v>
       </c>
       <c r="D6">
         <v>1.2</v>
@@ -2179,7 +2286,7 @@
       </c>
       <c r="C7" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.0299999999999998</v>
+        <v>2.56</v>
       </c>
       <c r="D7">
         <v>2</v>
@@ -2195,7 +2302,7 @@
       </c>
       <c r="C8" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.79</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -2208,7 +2315,7 @@
       </c>
       <c r="C9" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.33</v>
+        <v>2.52</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -2224,7 +2331,7 @@
       </c>
       <c r="C10" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.74</v>
+        <v>2.56</v>
       </c>
       <c r="D10">
         <v>1.2</v>
@@ -2240,7 +2347,7 @@
       </c>
       <c r="C11" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.38</v>
+        <v>2.16</v>
       </c>
       <c r="D11">
         <v>2</v>
@@ -2256,7 +2363,7 @@
       </c>
       <c r="C12" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.69</v>
+        <v>0.83</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -2269,10 +2376,41 @@
       </c>
       <c r="C13" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.53</v>
+        <v>0.67</v>
       </c>
       <c r="D13">
         <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14">
+        <v>1.2</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Joint factor was added to file.
</commit_message>
<xml_diff>
--- a/Mosquito/mosdb.xlsx
+++ b/Mosquito/mosdb.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="15315" windowHeight="6210" activeTab="5"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="15315" windowHeight="6210" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Системы" sheetId="10" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="104">
   <si>
     <t>Имя</t>
   </si>
@@ -336,6 +336,12 @@
   </si>
   <si>
     <t>Заклёпки (шт)</t>
+  </si>
+  <si>
+    <t>Наличие паза</t>
+  </si>
+  <si>
+    <t>+</t>
   </si>
 </sst>
 </file>
@@ -776,7 +782,7 @@
       </c>
       <c r="C2" s="2">
         <f t="shared" ref="C2:C25" ca="1" si="0">RANDBETWEEN(50,300)/100</f>
-        <v>2.84</v>
+        <v>0.83</v>
       </c>
       <c r="D2">
         <v>1.2</v>
@@ -792,7 +798,7 @@
       </c>
       <c r="C3" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.31</v>
+        <v>2.89</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -808,7 +814,7 @@
       </c>
       <c r="C4" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.1</v>
+        <v>2.14</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -824,7 +830,7 @@
       </c>
       <c r="C5" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.4</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -840,7 +846,7 @@
       </c>
       <c r="C6" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.99</v>
+        <v>2.13</v>
       </c>
       <c r="D6">
         <v>1.2</v>
@@ -856,7 +862,7 @@
       </c>
       <c r="C7" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.14</v>
+        <v>2.97</v>
       </c>
       <c r="D7">
         <v>2</v>
@@ -872,7 +878,7 @@
       </c>
       <c r="C8" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.82</v>
+        <v>2.9</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -885,7 +891,7 @@
       </c>
       <c r="C9" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.91</v>
+        <v>1.77</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -901,7 +907,7 @@
       </c>
       <c r="C10" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.83</v>
+        <v>1.29</v>
       </c>
       <c r="D10">
         <v>1.2</v>
@@ -917,7 +923,7 @@
       </c>
       <c r="C11" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.72</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="D11">
         <v>2</v>
@@ -933,7 +939,7 @@
       </c>
       <c r="C12" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.64</v>
+        <v>1.43</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -946,7 +952,7 @@
       </c>
       <c r="C13" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.97</v>
+        <v>2.77</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -962,7 +968,7 @@
       </c>
       <c r="C14" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.63</v>
+        <v>1.34</v>
       </c>
       <c r="D14">
         <v>1.2</v>
@@ -978,7 +984,7 @@
       </c>
       <c r="C15" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.85</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="D15">
         <v>2</v>
@@ -994,7 +1000,7 @@
       </c>
       <c r="C16" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.95</v>
+        <v>1.63</v>
       </c>
       <c r="D16">
         <v>2</v>
@@ -1010,7 +1016,7 @@
       </c>
       <c r="C17" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.65</v>
+        <v>2.11</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -1026,7 +1032,7 @@
       </c>
       <c r="C18" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.75</v>
+        <v>0.59</v>
       </c>
       <c r="D18">
         <v>1.2</v>
@@ -1042,7 +1048,7 @@
       </c>
       <c r="C19" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.39</v>
+        <v>2.29</v>
       </c>
       <c r="D19">
         <v>2</v>
@@ -1058,7 +1064,7 @@
       </c>
       <c r="C20" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.26</v>
+        <v>1.32</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1071,7 +1077,7 @@
       </c>
       <c r="C21" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.5</v>
+        <v>2.2799999999999998</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -1087,7 +1093,7 @@
       </c>
       <c r="C22" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.8</v>
+        <v>2.83</v>
       </c>
       <c r="D22">
         <v>1.2</v>
@@ -1103,7 +1109,7 @@
       </c>
       <c r="C23" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.61</v>
+        <v>2.7</v>
       </c>
       <c r="D23">
         <v>2</v>
@@ -1119,7 +1125,7 @@
       </c>
       <c r="C24" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.67</v>
+        <v>2.87</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1131,7 +1137,7 @@
       </c>
       <c r="C25" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.0499999999999998</v>
+        <v>2.37</v>
       </c>
       <c r="D25">
         <v>2</v>
@@ -1150,7 +1156,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1438,10 +1444,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="E1" sqref="E1:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1449,9 +1455,10 @@
     <col min="2" max="2" width="46.85546875" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
     <col min="4" max="4" width="17.28515625" customWidth="1"/>
+    <col min="5" max="5" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>91</v>
       </c>
@@ -1464,8 +1471,11 @@
       <c r="D1" s="3" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1478,8 +1488,11 @@
       <c r="D2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1492,8 +1505,11 @@
       <c r="D3">
         <v>1.2</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1507,7 +1523,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1518,7 +1534,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
     </row>
@@ -1837,7 +1853,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
@@ -1899,7 +1915,7 @@
       </c>
       <c r="C3" s="2">
         <f t="shared" ref="C3:C5" ca="1" si="0">RANDBETWEEN(50,300)/100</f>
-        <v>2.59</v>
+        <v>2.85</v>
       </c>
       <c r="D3">
         <v>1.2</v>
@@ -1920,7 +1936,7 @@
       </c>
       <c r="C4" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.9</v>
+        <v>1.57</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -1941,7 +1957,7 @@
       </c>
       <c r="C5" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.6</v>
+        <v>0.87</v>
       </c>
       <c r="E5">
         <v>4</v>
@@ -1959,7 +1975,7 @@
       </c>
       <c r="C6" s="2">
         <f ca="1">RANDBETWEEN(50,300)/100</f>
-        <v>1.87</v>
+        <v>2.2599999999999998</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -1980,7 +1996,7 @@
       </c>
       <c r="C7" s="2">
         <f ca="1">RANDBETWEEN(50,300)/100</f>
-        <v>2.2200000000000002</v>
+        <v>2.84</v>
       </c>
       <c r="D7">
         <v>1.2</v>
@@ -2001,7 +2017,7 @@
       </c>
       <c r="C8" s="2">
         <f ca="1">RANDBETWEEN(50,300)/100</f>
-        <v>1.68</v>
+        <v>1.63</v>
       </c>
       <c r="D8">
         <v>2</v>
@@ -2056,7 +2072,7 @@
       </c>
       <c r="C2" s="2">
         <f ca="1">RANDBETWEEN(50,300)/100</f>
-        <v>2.5099999999999998</v>
+        <v>2.9</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -2071,7 +2087,7 @@
       </c>
       <c r="C3" s="2">
         <f ca="1">RANDBETWEEN(50,300)/100</f>
-        <v>2.68</v>
+        <v>1.49</v>
       </c>
       <c r="D3">
         <v>1.2</v>
@@ -2086,7 +2102,7 @@
       </c>
       <c r="C4" s="2">
         <f ca="1">RANDBETWEEN(50,300)/100</f>
-        <v>2.67</v>
+        <v>1.83</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -2101,7 +2117,7 @@
       </c>
       <c r="C5" s="2">
         <f ca="1">RANDBETWEEN(50,300)/100</f>
-        <v>2.95</v>
+        <v>2.2599999999999998</v>
       </c>
     </row>
   </sheetData>
@@ -2111,19 +2127,20 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="42.28515625" customWidth="1"/>
     <col min="3" max="4" width="17.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>91</v>
       </c>
@@ -2136,8 +2153,11 @@
       <c r="D1" s="3" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2150,8 +2170,11 @@
       <c r="D2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2160,7 +2183,7 @@
       </c>
       <c r="C3" s="2">
         <f ca="1">RANDBETWEEN(50,300)/100</f>
-        <v>2.66</v>
+        <v>1.22</v>
       </c>
       <c r="D3">
         <v>1.2</v>
@@ -2209,7 +2232,7 @@
       </c>
       <c r="C2" s="2">
         <f t="shared" ref="C2:C13" ca="1" si="0">RANDBETWEEN(50,300)/100</f>
-        <v>2.96</v>
+        <v>0.67</v>
       </c>
       <c r="D2">
         <v>1.2</v>
@@ -2225,7 +2248,7 @@
       </c>
       <c r="C3" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.95</v>
+        <v>2.52</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -2241,7 +2264,7 @@
       </c>
       <c r="C4" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.77</v>
+        <v>2.44</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2254,7 +2277,7 @@
       </c>
       <c r="C5" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.75</v>
+        <v>1.95</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -2270,7 +2293,7 @@
       </c>
       <c r="C6" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.42</v>
+        <v>2.7</v>
       </c>
       <c r="D6">
         <v>1.2</v>
@@ -2286,7 +2309,7 @@
       </c>
       <c r="C7" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.56</v>
+        <v>0.92</v>
       </c>
       <c r="D7">
         <v>2</v>
@@ -2302,7 +2325,7 @@
       </c>
       <c r="C8" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.51</v>
+        <v>1.97</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -2315,7 +2338,7 @@
       </c>
       <c r="C9" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.52</v>
+        <v>1.72</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -2331,7 +2354,7 @@
       </c>
       <c r="C10" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.56</v>
+        <v>2.4300000000000002</v>
       </c>
       <c r="D10">
         <v>1.2</v>
@@ -2347,7 +2370,7 @@
       </c>
       <c r="C11" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.16</v>
+        <v>1.58</v>
       </c>
       <c r="D11">
         <v>2</v>
@@ -2363,7 +2386,7 @@
       </c>
       <c r="C12" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.83</v>
+        <v>1.83</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -2376,7 +2399,7 @@
       </c>
       <c r="C13" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.67</v>
+        <v>0.75</v>
       </c>
       <c r="D13">
         <v>1</v>

</xml_diff>

<commit_message>
Mount product was extended.
</commit_message>
<xml_diff>
--- a/Mosquito/mosdb.xlsx
+++ b/Mosquito/mosdb.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="15315" windowHeight="6210" firstSheet="1" activeTab="7"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="15315" windowHeight="6210" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Системы" sheetId="10" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="104">
   <si>
     <t>Имя</t>
   </si>
@@ -782,7 +782,7 @@
       </c>
       <c r="C2" s="2">
         <f t="shared" ref="C2:C25" ca="1" si="0">RANDBETWEEN(50,300)/100</f>
-        <v>0.83</v>
+        <v>1.93</v>
       </c>
       <c r="D2">
         <v>1.2</v>
@@ -798,7 +798,7 @@
       </c>
       <c r="C3" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.89</v>
+        <v>1.07</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -814,7 +814,7 @@
       </c>
       <c r="C4" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.14</v>
+        <v>2.81</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -830,7 +830,7 @@
       </c>
       <c r="C5" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.1200000000000001</v>
+        <v>0.78</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -846,7 +846,7 @@
       </c>
       <c r="C6" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.13</v>
+        <v>1.38</v>
       </c>
       <c r="D6">
         <v>1.2</v>
@@ -862,7 +862,7 @@
       </c>
       <c r="C7" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.97</v>
+        <v>0.91</v>
       </c>
       <c r="D7">
         <v>2</v>
@@ -878,7 +878,7 @@
       </c>
       <c r="C8" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.9</v>
+        <v>2.68</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -891,7 +891,7 @@
       </c>
       <c r="C9" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.77</v>
+        <v>2.72</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -907,7 +907,7 @@
       </c>
       <c r="C10" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.29</v>
+        <v>1.68</v>
       </c>
       <c r="D10">
         <v>1.2</v>
@@ -923,7 +923,7 @@
       </c>
       <c r="C11" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.56000000000000005</v>
+        <v>1.58</v>
       </c>
       <c r="D11">
         <v>2</v>
@@ -939,7 +939,7 @@
       </c>
       <c r="C12" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.43</v>
+        <v>0.79</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -952,7 +952,7 @@
       </c>
       <c r="C13" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.77</v>
+        <v>1.37</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -968,7 +968,7 @@
       </c>
       <c r="C14" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.34</v>
+        <v>0.87</v>
       </c>
       <c r="D14">
         <v>1.2</v>
@@ -984,7 +984,7 @@
       </c>
       <c r="C15" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.1599999999999999</v>
+        <v>2.66</v>
       </c>
       <c r="D15">
         <v>2</v>
@@ -1000,7 +1000,7 @@
       </c>
       <c r="C16" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.63</v>
+        <v>1.31</v>
       </c>
       <c r="D16">
         <v>2</v>
@@ -1016,7 +1016,7 @@
       </c>
       <c r="C17" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.11</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -1032,7 +1032,7 @@
       </c>
       <c r="C18" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.59</v>
+        <v>1.35</v>
       </c>
       <c r="D18">
         <v>1.2</v>
@@ -1048,7 +1048,7 @@
       </c>
       <c r="C19" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.29</v>
+        <v>1.59</v>
       </c>
       <c r="D19">
         <v>2</v>
@@ -1064,7 +1064,7 @@
       </c>
       <c r="C20" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.32</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1077,7 +1077,7 @@
       </c>
       <c r="C21" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.2799999999999998</v>
+        <v>0.74</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -1093,7 +1093,7 @@
       </c>
       <c r="C22" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.83</v>
+        <v>2.1800000000000002</v>
       </c>
       <c r="D22">
         <v>1.2</v>
@@ -1109,7 +1109,7 @@
       </c>
       <c r="C23" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.7</v>
+        <v>2.3199999999999998</v>
       </c>
       <c r="D23">
         <v>2</v>
@@ -1125,7 +1125,7 @@
       </c>
       <c r="C24" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.87</v>
+        <v>1.29</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1137,7 +1137,7 @@
       </c>
       <c r="C25" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.37</v>
+        <v>0.76</v>
       </c>
       <c r="D25">
         <v>2</v>
@@ -1854,7 +1854,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="E1" sqref="E1:F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1915,7 +1915,7 @@
       </c>
       <c r="C3" s="2">
         <f t="shared" ref="C3:C5" ca="1" si="0">RANDBETWEEN(50,300)/100</f>
-        <v>2.85</v>
+        <v>1.29</v>
       </c>
       <c r="D3">
         <v>1.2</v>
@@ -1936,7 +1936,7 @@
       </c>
       <c r="C4" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.57</v>
+        <v>0.6</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -1957,7 +1957,7 @@
       </c>
       <c r="C5" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.87</v>
+        <v>2.5499999999999998</v>
       </c>
       <c r="E5">
         <v>4</v>
@@ -1975,7 +1975,7 @@
       </c>
       <c r="C6" s="2">
         <f ca="1">RANDBETWEEN(50,300)/100</f>
-        <v>2.2599999999999998</v>
+        <v>0.8</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -1996,7 +1996,7 @@
       </c>
       <c r="C7" s="2">
         <f ca="1">RANDBETWEEN(50,300)/100</f>
-        <v>2.84</v>
+        <v>2.09</v>
       </c>
       <c r="D7">
         <v>1.2</v>
@@ -2017,7 +2017,7 @@
       </c>
       <c r="C8" s="2">
         <f ca="1">RANDBETWEEN(50,300)/100</f>
-        <v>1.63</v>
+        <v>1.84</v>
       </c>
       <c r="D8">
         <v>2</v>
@@ -2036,10 +2036,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2047,9 +2047,11 @@
     <col min="2" max="2" width="48.7109375" customWidth="1"/>
     <col min="3" max="3" width="15.42578125" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>91</v>
       </c>
@@ -2062,8 +2064,14 @@
       <c r="D1" s="3" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2072,13 +2080,19 @@
       </c>
       <c r="C2" s="2">
         <f ca="1">RANDBETWEEN(50,300)/100</f>
-        <v>2.9</v>
+        <v>2.98</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>4</v>
+      </c>
+      <c r="F2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2087,13 +2101,19 @@
       </c>
       <c r="C3" s="2">
         <f ca="1">RANDBETWEEN(50,300)/100</f>
-        <v>1.49</v>
+        <v>1.86</v>
       </c>
       <c r="D3">
         <v>1.2</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>4</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2102,13 +2122,19 @@
       </c>
       <c r="C4" s="2">
         <f ca="1">RANDBETWEEN(50,300)/100</f>
-        <v>1.83</v>
+        <v>1.01</v>
       </c>
       <c r="D4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2117,7 +2143,37 @@
       </c>
       <c r="C5" s="2">
         <f ca="1">RANDBETWEEN(50,300)/100</f>
-        <v>2.2599999999999998</v>
+        <v>1.25</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>4</v>
+      </c>
+      <c r="F7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>4</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2129,7 +2185,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -2183,7 +2239,7 @@
       </c>
       <c r="C3" s="2">
         <f ca="1">RANDBETWEEN(50,300)/100</f>
-        <v>1.22</v>
+        <v>1.54</v>
       </c>
       <c r="D3">
         <v>1.2</v>
@@ -2232,7 +2288,7 @@
       </c>
       <c r="C2" s="2">
         <f t="shared" ref="C2:C13" ca="1" si="0">RANDBETWEEN(50,300)/100</f>
-        <v>0.67</v>
+        <v>2.97</v>
       </c>
       <c r="D2">
         <v>1.2</v>
@@ -2248,7 +2304,7 @@
       </c>
       <c r="C3" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.52</v>
+        <v>2.17</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -2264,7 +2320,7 @@
       </c>
       <c r="C4" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.44</v>
+        <v>0.53</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2277,7 +2333,7 @@
       </c>
       <c r="C5" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.95</v>
+        <v>2.27</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -2293,7 +2349,7 @@
       </c>
       <c r="C6" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.7</v>
+        <v>1.62</v>
       </c>
       <c r="D6">
         <v>1.2</v>
@@ -2309,7 +2365,7 @@
       </c>
       <c r="C7" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.92</v>
+        <v>1.23</v>
       </c>
       <c r="D7">
         <v>2</v>
@@ -2325,7 +2381,7 @@
       </c>
       <c r="C8" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.97</v>
+        <v>2.88</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -2338,7 +2394,7 @@
       </c>
       <c r="C9" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.72</v>
+        <v>1.22</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -2354,7 +2410,7 @@
       </c>
       <c r="C10" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.4300000000000002</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="D10">
         <v>1.2</v>
@@ -2370,7 +2426,7 @@
       </c>
       <c r="C11" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.58</v>
+        <v>0.73</v>
       </c>
       <c r="D11">
         <v>2</v>
@@ -2386,7 +2442,7 @@
       </c>
       <c r="C12" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1.83</v>
+        <v>2.19</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -2399,7 +2455,7 @@
       </c>
       <c r="C13" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.75</v>
+        <v>0.59</v>
       </c>
       <c r="D13">
         <v>1</v>

</xml_diff>